<commit_message>
Güncellenmiş STO_Planner kodları eklendi
</commit_message>
<xml_diff>
--- a/material.xlsx
+++ b/material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trkizilkbu\STO_Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5B8780-488F-4292-80A3-9127291E3041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660E35D5-3807-4E0F-A911-3BFFC6E1A656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5396C47A-4C1D-4DB1-A47A-ABBEDD339A8F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3042" uniqueCount="1027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3069" uniqueCount="1037">
   <si>
     <t>Material Description</t>
   </si>
@@ -3117,6 +3117,36 @@
   </si>
   <si>
     <t>Kısa Hafif Palet</t>
+  </si>
+  <si>
+    <t>GERBER Org PorrAppPmpkCarrot8x110g N1 TR</t>
+  </si>
+  <si>
+    <t>GERBER Org Porridge AppMango8x110g N1 TR</t>
+  </si>
+  <si>
+    <t>NC 3IN1 Ice Choco MP 12(10x10.6g) RG TR</t>
+  </si>
+  <si>
+    <t>NC 3IN1 10(56x17.5g) RG TR</t>
+  </si>
+  <si>
+    <t>NESCAFE GOLD Jar 6x200g N3 TR</t>
+  </si>
+  <si>
+    <t>NESQUIK Cereal Bar Dspl 9(24x25g) N5 TR</t>
+  </si>
+  <si>
+    <t>NESCAFE CLASSIC FINE BLEND DSC 12x70g TR</t>
+  </si>
+  <si>
+    <t>NESFIT GNLACRAN CerBag 7x300g N52TF TR</t>
+  </si>
+  <si>
+    <t>NESQUIK Strawberry Pouch 14x350g N2 DE</t>
+  </si>
+  <si>
+    <t>Kısa Ağır Palet</t>
   </si>
 </sst>
 </file>
@@ -3245,7 +3275,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3287,12 +3317,26 @@
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3779,21 +3823,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFE8FCC4-913C-458E-B624-765861CC15FD}" name="Table_query__14" displayName="Table_query__14" ref="A1:L1011" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="13">
-  <autoFilter ref="A1:L1011" xr:uid="{DFE8FCC4-913C-458E-B624-765861CC15FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFE8FCC4-913C-458E-B624-765861CC15FD}" name="Table_query__14" displayName="Table_query__14" ref="A1:L1020" totalsRowShown="0" headerRowDxfId="18" dataDxfId="16" headerRowBorderDxfId="17" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A1:L1020" xr:uid="{DFE8FCC4-913C-458E-B624-765861CC15FD}"/>
   <tableColumns count="12">
-    <tableColumn id="2" xr3:uid="{EA02FFB0-F0E0-4ED8-BC6D-48C33AF3755A}" name="Material" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{EA1F3D64-78F4-4546-9F67-8804A37FC7EF}" name="Material Description" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{FB761F83-67D3-4DF3-AF05-80569C9D11B4}" name="CS/LAY" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{21D1DA3D-991D-406E-ABED-783914DEF0DF}" name="CS/PAL" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{5A4F5DD9-7587-4258-BFF8-C52DD378F5D6}" name="CS_Height_CM" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{D88B5A6B-1A4F-43A9-9457-654946A0CFF9}" name="CS_Volume_M3" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{5363A2AA-29ED-4F40-930B-1F9729976839}" name="CS_Weight_KG" dataDxfId="6" dataCellStyle="Comma"/>
-    <tableColumn id="9" xr3:uid="{B4089EC7-F383-475A-846F-FE9904776411}" name="Temp_Type" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{BF38389B-5A7C-4CA1-9CE5-08E7F324A889}" name="PALTypeChoice" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{212ADAD0-7A1F-4D96-9767-5BEE6FC601A4}" name="Pallet_Height" dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="1" xr3:uid="{1B3C5978-A2E6-46D6-B207-FE432D8A7B9A}" name="Pallet_Gross" dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="12" xr3:uid="{8ABC39E9-5F14-4ACC-97ED-C535CA201E69}" name="Pallet_M3" dataDxfId="1" dataCellStyle="Comma"/>
+    <tableColumn id="2" xr3:uid="{EA02FFB0-F0E0-4ED8-BC6D-48C33AF3755A}" name="Material" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{EA1F3D64-78F4-4546-9F67-8804A37FC7EF}" name="Material Description" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{FB761F83-67D3-4DF3-AF05-80569C9D11B4}" name="CS/LAY" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{21D1DA3D-991D-406E-ABED-783914DEF0DF}" name="CS/PAL" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{5A4F5DD9-7587-4258-BFF8-C52DD378F5D6}" name="CS_Height_CM" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{D88B5A6B-1A4F-43A9-9457-654946A0CFF9}" name="CS_Volume_M3" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{5363A2AA-29ED-4F40-930B-1F9729976839}" name="CS_Weight_KG" dataDxfId="7" dataCellStyle="Comma"/>
+    <tableColumn id="9" xr3:uid="{B4089EC7-F383-475A-846F-FE9904776411}" name="Temp_Type" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{BF38389B-5A7C-4CA1-9CE5-08E7F324A889}" name="PALTypeChoice" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{212ADAD0-7A1F-4D96-9767-5BEE6FC601A4}" name="Pallet_Height" dataDxfId="4" dataCellStyle="Comma"/>
+    <tableColumn id="1" xr3:uid="{1B3C5978-A2E6-46D6-B207-FE432D8A7B9A}" name="Pallet_Gross" dataDxfId="3" dataCellStyle="Comma"/>
+    <tableColumn id="12" xr3:uid="{8ABC39E9-5F14-4ACC-97ED-C535CA201E69}" name="Pallet_M3" dataDxfId="2" dataCellStyle="Comma"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4116,10 +4160,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A631398A-BE09-4A20-AAB4-BDD71B16571E}">
-  <dimension ref="A1:L1057"/>
+  <dimension ref="A1:L1054"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1001" workbookViewId="0">
-      <selection activeCell="F1018" sqref="F1018"/>
+    <sheetView tabSelected="1" topLeftCell="A1001" workbookViewId="0">
+      <selection activeCell="D1021" sqref="D1021"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.08984375" defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
@@ -42552,125 +42596,347 @@
         <v>1.8720000000000001</v>
       </c>
     </row>
-    <row r="1012" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1012"/>
-      <c r="B1012"/>
-      <c r="C1012"/>
-      <c r="D1012"/>
-      <c r="E1012"/>
-      <c r="F1012"/>
-      <c r="G1012"/>
-      <c r="H1012"/>
-      <c r="I1012"/>
-      <c r="J1012"/>
-      <c r="K1012"/>
-      <c r="L1012"/>
-    </row>
-    <row r="1013" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1013"/>
-      <c r="B1013"/>
-      <c r="C1013"/>
-      <c r="D1013"/>
-      <c r="E1013"/>
-      <c r="F1013"/>
-      <c r="G1013"/>
-      <c r="H1013"/>
-      <c r="I1013"/>
-      <c r="J1013"/>
-      <c r="K1013"/>
-      <c r="L1013"/>
-    </row>
-    <row r="1014" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1014"/>
-      <c r="B1014"/>
-      <c r="C1014"/>
-      <c r="D1014"/>
-      <c r="E1014"/>
-      <c r="F1014"/>
-      <c r="G1014"/>
-      <c r="H1014"/>
-      <c r="I1014"/>
-      <c r="J1014"/>
-      <c r="K1014"/>
-      <c r="L1014"/>
-    </row>
-    <row r="1015" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1015"/>
-      <c r="B1015"/>
-      <c r="C1015"/>
-      <c r="D1015"/>
-      <c r="E1015"/>
-      <c r="F1015"/>
-      <c r="G1015"/>
-      <c r="H1015"/>
-      <c r="I1015"/>
-      <c r="J1015"/>
-      <c r="K1015"/>
-      <c r="L1015"/>
-    </row>
-    <row r="1016" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1016"/>
-      <c r="B1016"/>
-      <c r="C1016"/>
-      <c r="D1016"/>
-      <c r="E1016"/>
-      <c r="F1016"/>
-      <c r="G1016"/>
-      <c r="H1016"/>
-      <c r="I1016"/>
-      <c r="J1016"/>
-      <c r="K1016"/>
-      <c r="L1016"/>
-    </row>
-    <row r="1017" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1017"/>
-      <c r="B1017"/>
-      <c r="C1017"/>
-      <c r="D1017"/>
-      <c r="E1017"/>
-      <c r="F1017"/>
-      <c r="G1017"/>
-      <c r="H1017"/>
-      <c r="I1017"/>
-      <c r="J1017"/>
-      <c r="K1017"/>
-      <c r="L1017"/>
-    </row>
-    <row r="1018" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1018"/>
-      <c r="B1018"/>
-      <c r="C1018"/>
-      <c r="D1018"/>
-      <c r="E1018"/>
-      <c r="F1018"/>
-      <c r="G1018" s="20"/>
-      <c r="H1018"/>
-      <c r="I1018"/>
-      <c r="J1018" s="20"/>
-    </row>
-    <row r="1019" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1019"/>
-      <c r="B1019"/>
-      <c r="C1019"/>
-      <c r="D1019"/>
-      <c r="E1019"/>
-      <c r="F1019"/>
-      <c r="G1019" s="20"/>
-      <c r="H1019"/>
-      <c r="I1019"/>
-      <c r="J1019" s="20"/>
-    </row>
-    <row r="1020" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1020"/>
-      <c r="B1020"/>
-      <c r="C1020"/>
-      <c r="D1020"/>
-      <c r="E1020"/>
-      <c r="F1020"/>
-      <c r="G1020" s="20"/>
-      <c r="H1020"/>
-      <c r="I1020"/>
-      <c r="J1020" s="20"/>
+    <row r="1012" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1012" s="31">
+        <v>12573197</v>
+      </c>
+      <c r="B1012" s="4" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C1012" s="5">
+        <v>15</v>
+      </c>
+      <c r="D1012" s="5">
+        <v>60</v>
+      </c>
+      <c r="E1012" s="5">
+        <v>24</v>
+      </c>
+      <c r="F1012" s="6">
+        <v>1.5359999999999999E-2</v>
+      </c>
+      <c r="G1012" s="32">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="H1012" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1012" s="7" t="s">
+        <v>1026</v>
+      </c>
+      <c r="J1012" s="21">
+        <v>111</v>
+      </c>
+      <c r="K1012" s="8">
+        <v>93</v>
+      </c>
+      <c r="L1012" s="22">
+        <v>1.0660000000000001</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1013" s="31">
+        <v>12585019</v>
+      </c>
+      <c r="B1013" s="4" t="s">
+        <v>1028</v>
+      </c>
+      <c r="C1013" s="5">
+        <v>38</v>
+      </c>
+      <c r="D1013" s="5">
+        <v>228</v>
+      </c>
+      <c r="E1013" s="5">
+        <v>17.2</v>
+      </c>
+      <c r="F1013" s="6">
+        <v>4.0350000000000004E-3</v>
+      </c>
+      <c r="G1013" s="32">
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="H1013" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1013" s="7" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J1013" s="21">
+        <v>118.2</v>
+      </c>
+      <c r="K1013" s="8">
+        <v>259</v>
+      </c>
+      <c r="L1013" s="22">
+        <v>1.135</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1014" s="31">
+        <v>12585057</v>
+      </c>
+      <c r="B1014" s="4" t="s">
+        <v>1027</v>
+      </c>
+      <c r="C1014" s="5">
+        <v>38</v>
+      </c>
+      <c r="D1014" s="5">
+        <v>228</v>
+      </c>
+      <c r="E1014" s="5">
+        <v>17.2</v>
+      </c>
+      <c r="F1014" s="6">
+        <v>4.0350000000000004E-3</v>
+      </c>
+      <c r="G1014" s="32">
+        <v>1.0229999999999999</v>
+      </c>
+      <c r="H1014" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1014" s="7" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J1014" s="21">
+        <v>118.2</v>
+      </c>
+      <c r="K1014" s="8">
+        <v>259</v>
+      </c>
+      <c r="L1014" s="22">
+        <v>1.135</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1015" s="31">
+        <v>12595303</v>
+      </c>
+      <c r="B1015" s="4" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C1015" s="5">
+        <v>19</v>
+      </c>
+      <c r="D1015" s="5">
+        <v>95</v>
+      </c>
+      <c r="E1015" s="5">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="F1015" s="6">
+        <v>8.8240000000000002E-3</v>
+      </c>
+      <c r="G1015" s="32">
+        <v>3.94</v>
+      </c>
+      <c r="H1015" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1015" s="7" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J1015" s="21">
+        <v>110.5</v>
+      </c>
+      <c r="K1015" s="8">
+        <v>400</v>
+      </c>
+      <c r="L1015" s="22">
+        <v>1.0609999999999999</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1016" s="31">
+        <v>12608119</v>
+      </c>
+      <c r="B1016" s="4" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C1016" s="5">
+        <v>8</v>
+      </c>
+      <c r="D1016" s="5">
+        <v>40</v>
+      </c>
+      <c r="E1016" s="5">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="F1016" s="6">
+        <v>1.9682999999999999E-2</v>
+      </c>
+      <c r="G1016" s="32">
+        <v>5.39</v>
+      </c>
+      <c r="H1016" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1016" s="7" t="s">
+        <v>1036</v>
+      </c>
+      <c r="J1016" s="21">
+        <v>103</v>
+      </c>
+      <c r="K1016" s="8">
+        <v>241</v>
+      </c>
+      <c r="L1016" s="22">
+        <v>0.9887999999999999</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1017" s="31">
+        <v>12608895</v>
+      </c>
+      <c r="B1017" s="4" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C1017" s="5">
+        <v>9</v>
+      </c>
+      <c r="D1017" s="5">
+        <v>63</v>
+      </c>
+      <c r="E1017" s="5">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="F1017" s="6">
+        <v>3.4055999999999996E-2</v>
+      </c>
+      <c r="G1017" s="32">
+        <v>7.2</v>
+      </c>
+      <c r="H1017" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1017" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1017" s="21">
+        <v>243.9</v>
+      </c>
+      <c r="K1017" s="8">
+        <v>480</v>
+      </c>
+      <c r="L1017" s="22">
+        <v>2.3410000000000002</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1018" s="31">
+        <v>12609324</v>
+      </c>
+      <c r="B1018" s="4" t="s">
+        <v>1030</v>
+      </c>
+      <c r="C1018" s="5">
+        <v>6</v>
+      </c>
+      <c r="D1018" s="5">
+        <v>30</v>
+      </c>
+      <c r="E1018" s="5">
+        <v>29.8</v>
+      </c>
+      <c r="F1018" s="6">
+        <v>4.2548000000000002E-2</v>
+      </c>
+      <c r="G1018" s="32">
+        <v>11.9</v>
+      </c>
+      <c r="H1018" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1018" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1018" s="21">
+        <v>164</v>
+      </c>
+      <c r="K1018" s="8">
+        <v>382</v>
+      </c>
+      <c r="L1018" s="22">
+        <v>1.5740000000000001</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1019" s="31">
+        <v>12609555</v>
+      </c>
+      <c r="B1019" s="4" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C1019" s="5">
+        <v>14</v>
+      </c>
+      <c r="D1019" s="5">
+        <v>140</v>
+      </c>
+      <c r="E1019" s="5">
+        <v>18.5</v>
+      </c>
+      <c r="F1019" s="6">
+        <v>1.1448E-2</v>
+      </c>
+      <c r="G1019" s="32">
+        <v>1.67</v>
+      </c>
+      <c r="H1019" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1019" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1019" s="21">
+        <v>200</v>
+      </c>
+      <c r="K1019" s="8">
+        <v>259</v>
+      </c>
+      <c r="L1019" s="22">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1020" s="33">
+        <v>12617734</v>
+      </c>
+      <c r="B1020" s="11" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C1020" s="12">
+        <v>12</v>
+      </c>
+      <c r="D1020" s="12">
+        <v>96</v>
+      </c>
+      <c r="E1020" s="12">
+        <v>21.2</v>
+      </c>
+      <c r="F1020" s="13">
+        <v>1.6663000000000001E-2</v>
+      </c>
+      <c r="G1020" s="34">
+        <v>2.41</v>
+      </c>
+      <c r="H1020" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1020" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1020" s="25">
+        <v>184.6</v>
+      </c>
+      <c r="K1020" s="14">
+        <v>257</v>
+      </c>
+      <c r="L1020" s="24">
+        <v>1.772</v>
+      </c>
     </row>
     <row r="1021" spans="1:12" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1021"/>
@@ -43080,45 +43346,9 @@
       <c r="I1054"/>
       <c r="J1054" s="20"/>
     </row>
-    <row r="1055" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1055"/>
-      <c r="B1055"/>
-      <c r="C1055"/>
-      <c r="D1055"/>
-      <c r="E1055"/>
-      <c r="F1055"/>
-      <c r="G1055" s="20"/>
-      <c r="H1055"/>
-      <c r="I1055"/>
-      <c r="J1055" s="20"/>
-    </row>
-    <row r="1056" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1056"/>
-      <c r="B1056"/>
-      <c r="C1056"/>
-      <c r="D1056"/>
-      <c r="E1056"/>
-      <c r="F1056"/>
-      <c r="G1056" s="20"/>
-      <c r="H1056"/>
-      <c r="I1056"/>
-      <c r="J1056" s="20"/>
-    </row>
-    <row r="1057" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1057"/>
-      <c r="B1057"/>
-      <c r="C1057"/>
-      <c r="D1057"/>
-      <c r="E1057"/>
-      <c r="F1057"/>
-      <c r="G1057" s="20"/>
-      <c r="H1057"/>
-      <c r="I1057"/>
-      <c r="J1057" s="20"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A1011">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  <conditionalFormatting sqref="A2:A1020">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>